<commit_message>
Task Scheduling Part1 Completed
...
</commit_message>
<xml_diff>
--- a/Document/Teamwork Cooperation/Task Scheduling.xlsx
+++ b/Document/Teamwork Cooperation/Task Scheduling.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="38400" windowHeight="19460"/>
+    <workbookView xWindow="920" yWindow="880" windowWidth="36160" windowHeight="18280"/>
   </bookViews>
   <sheets>
     <sheet name="任务" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>任务列表</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -89,193 +89,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1.框架应将项目基本Gameplay所需的基类、接口、委托等进行初步的代码实现；
-2.框架应具备适当的易用性，即框架的学习使用成本，不应占用过多的项目开发时间；
-3.在保证前2点的前提下，尽可能地减少框架本身的BUG，尽可能将框架设计的更加优雅，可拓展性、可维护性更高。
-1.The framework should carry out preliminary code implementation of the basic classes, interfaces, and delegates required for the basic Gameplay of the project;
-2.The framework should be easy to use, the cost of  framework learning should not take up too much project development time;
-3.In the premise of ensuring the first 2 points, you can reduce the BUG of the frame as much as possible, and make the frame more elegant, extensibility and maintainability as far as possible。
-</t>
-    <rPh sb="2" eb="3">
-      <t>kuang'j</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>ying</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>jiang</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>xiang'mu</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ji'ben</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>suo'xu</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>de</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>ji'lei</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>jie'kou</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>wei'tuo</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>deng</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>jin'xing</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>chu'bu</t>
-    </rPh>
-    <rPh sb="34" eb="35">
-      <t>de</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>dai'm</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>shi'xian</t>
-    </rPh>
-    <rPh sb="43" eb="44">
-      <t>kuang'j</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>ying'ju'bei</t>
-    </rPh>
-    <rPh sb="48" eb="49">
-      <t>shi'dang</t>
-    </rPh>
-    <rPh sb="50" eb="51">
-      <t>de</t>
-    </rPh>
-    <rPh sb="51" eb="52">
-      <t>yi'yong'xing</t>
-    </rPh>
-    <rPh sb="55" eb="56">
-      <t>ji</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>kuang'j</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>de</t>
-    </rPh>
-    <rPh sb="59" eb="60">
-      <t>xue'xi</t>
-    </rPh>
-    <rPh sb="61" eb="62">
-      <t>shi'yong</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>cheng'b</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>bu'ying</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>zhan'yong</t>
-    </rPh>
-    <rPh sb="70" eb="71">
-      <t>guo'gao</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>duo</t>
-    </rPh>
-    <rPh sb="72" eb="73">
-      <t>de</t>
-    </rPh>
-    <rPh sb="73" eb="74">
-      <t>xiang'mu</t>
-    </rPh>
-    <rPh sb="75" eb="76">
-      <t>kai'fa</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>shi'jian</t>
-    </rPh>
-    <rPh sb="83" eb="84">
-      <t>zai</t>
-    </rPh>
-    <rPh sb="84" eb="85">
-      <t>bao'zheng</t>
-    </rPh>
-    <rPh sb="86" eb="87">
-      <t>qian</t>
-    </rPh>
-    <rPh sb="88" eb="89">
-      <t>dian</t>
-    </rPh>
-    <rPh sb="89" eb="90">
-      <t>de</t>
-    </rPh>
-    <rPh sb="90" eb="91">
-      <t>qian'ti</t>
-    </rPh>
-    <rPh sb="92" eb="93">
-      <t>xia</t>
-    </rPh>
-    <rPh sb="94" eb="95">
-      <t>jin'ke'negn</t>
-    </rPh>
-    <rPh sb="97" eb="98">
-      <t>di</t>
-    </rPh>
-    <rPh sb="98" eb="99">
-      <t>jian'shao</t>
-    </rPh>
-    <rPh sb="100" eb="101">
-      <t>kuang'j</t>
-    </rPh>
-    <rPh sb="102" eb="103">
-      <t>ben's</t>
-    </rPh>
-    <rPh sb="104" eb="105">
-      <t>de</t>
-    </rPh>
-    <rPh sb="109" eb="110">
-      <t>jin'ke'neng</t>
-    </rPh>
-    <rPh sb="112" eb="113">
-      <t>jiang</t>
-    </rPh>
-    <rPh sb="113" eb="114">
-      <t>kuang'j</t>
-    </rPh>
-    <rPh sb="115" eb="116">
-      <t>she'ji</t>
-    </rPh>
-    <rPh sb="117" eb="118">
-      <t>de</t>
-    </rPh>
-    <rPh sb="118" eb="119">
-      <t>geng'jia</t>
-    </rPh>
-    <rPh sb="120" eb="121">
-      <t>you'ya</t>
-    </rPh>
-    <rPh sb="123" eb="124">
-      <t>ke'tuo'zhan'x</t>
-    </rPh>
-    <rPh sb="128" eb="129">
-      <t>ke'wei'hu'x</t>
-    </rPh>
-    <rPh sb="132" eb="133">
-      <t>geng</t>
-    </rPh>
-    <rPh sb="133" eb="134">
-      <t>gao</t>
-    </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>游戏框架开发/Frame construction development</t>
     <rPh sb="0" eb="1">
       <t>you'xi</t>
@@ -1781,277 +1594,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1.框选之后按特定的组合键，能够进行编队，比如框选之后按ctrl+1，那么这次框选的游戏单位，将会被记录为1队，那么不管框选结束还是重新框选，当玩家再次按下1键时，会自动为玩家选择编队1的现存单位，并自动让这些单位变为已选状态;
-2.尽量保证功能的拓展性，比如组合键的可配置性，编队的队伍总量上限，每个队伍同时容纳的单位上限等相关逻辑参数，应该保证一定的灵活性。
-1.After finish selection and enter the specific key combination, game units can be teaming. Such press CTRL + 1, the game units that are selected, will be mark down as team1. Nomater ending selection or reselection, player can always call team 1 by press the key 1 key, automatically select the team1 for player.
-</t>
-    <rPh sb="2" eb="3">
-      <t>kuang'xuan</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>zhi'h</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>an</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>te'ding</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>de</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>zu'he'jian</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>neng</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>gou</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>jin'xing</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>bian'dui</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>bi'ru</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>kuang'xuan</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>zhi'h</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>an</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>na'm</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>zhe'ci</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>kuang'xuan</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>de</t>
-    </rPh>
-    <rPh sb="42" eb="43">
-      <t>you'xi</t>
-    </rPh>
-    <rPh sb="44" eb="45">
-      <t>dan'wei</t>
-    </rPh>
-    <rPh sb="47" eb="48">
-      <t>jiang</t>
-    </rPh>
-    <rPh sb="48" eb="49">
-      <t>hui</t>
-    </rPh>
-    <rPh sb="49" eb="50">
-      <t>bei</t>
-    </rPh>
-    <rPh sb="50" eb="51">
-      <t>ji'lu</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>wei</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>dui</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>na'm</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>bu'guan</t>
-    </rPh>
-    <rPh sb="60" eb="61">
-      <t>kuang'x</t>
-    </rPh>
-    <rPh sb="62" eb="63">
-      <t>jie'shu</t>
-    </rPh>
-    <rPh sb="64" eb="65">
-      <t>hai's</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>chogn'xin</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>kuang'x</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>dang</t>
-    </rPh>
-    <rPh sb="72" eb="73">
-      <t>wan'jia</t>
-    </rPh>
-    <rPh sb="74" eb="75">
-      <t>zai'ci</t>
-    </rPh>
-    <rPh sb="76" eb="77">
-      <t>an'xia</t>
-    </rPh>
-    <rPh sb="79" eb="80">
-      <t>jian</t>
-    </rPh>
-    <rPh sb="80" eb="81">
-      <t>shi</t>
-    </rPh>
-    <rPh sb="82" eb="83">
-      <t>hui</t>
-    </rPh>
-    <rPh sb="83" eb="84">
-      <t>zi'dong</t>
-    </rPh>
-    <rPh sb="85" eb="86">
-      <t>wei</t>
-    </rPh>
-    <rPh sb="86" eb="87">
-      <t>wan'jia</t>
-    </rPh>
-    <rPh sb="88" eb="89">
-      <t>xuan'z</t>
-    </rPh>
-    <rPh sb="90" eb="91">
-      <t>bian'dui</t>
-    </rPh>
-    <rPh sb="93" eb="94">
-      <t>de</t>
-    </rPh>
-    <rPh sb="94" eb="95">
-      <t>xian'cun</t>
-    </rPh>
-    <rPh sb="96" eb="97">
-      <t>dan'wei</t>
-    </rPh>
-    <rPh sb="99" eb="100">
-      <t>bing</t>
-    </rPh>
-    <rPh sb="100" eb="101">
-      <t>zi'dong</t>
-    </rPh>
-    <rPh sb="102" eb="103">
-      <t>rtang</t>
-    </rPh>
-    <rPh sb="103" eb="104">
-      <t>zhe'x</t>
-    </rPh>
-    <rPh sb="105" eb="106">
-      <t>dan'wei</t>
-    </rPh>
-    <rPh sb="107" eb="108">
-      <t>bian'wei</t>
-    </rPh>
-    <rPh sb="109" eb="110">
-      <t>yi</t>
-    </rPh>
-    <rPh sb="110" eb="111">
-      <t>xuan</t>
-    </rPh>
-    <rPh sb="111" eb="112">
-      <t>zhuang'tai</t>
-    </rPh>
-    <rPh sb="117" eb="118">
-      <t>jin'l</t>
-    </rPh>
-    <rPh sb="119" eb="120">
-      <t>bao'zheng</t>
-    </rPh>
-    <rPh sb="121" eb="122">
-      <t>gogn'n</t>
-    </rPh>
-    <rPh sb="123" eb="124">
-      <t>de</t>
-    </rPh>
-    <rPh sb="124" eb="125">
-      <t>tuo'zhan</t>
-    </rPh>
-    <rPh sb="126" eb="127">
-      <t>xing</t>
-    </rPh>
-    <rPh sb="128" eb="129">
-      <t>bi'ru</t>
-    </rPh>
-    <rPh sb="130" eb="131">
-      <t>zu'he'j</t>
-    </rPh>
-    <rPh sb="133" eb="134">
-      <t>de</t>
-    </rPh>
-    <rPh sb="134" eb="135">
-      <t>ke'pei'zhi'xing</t>
-    </rPh>
-    <rPh sb="139" eb="140">
-      <t>bian'dui</t>
-    </rPh>
-    <rPh sb="141" eb="142">
-      <t>de</t>
-    </rPh>
-    <rPh sb="142" eb="143">
-      <t>dui'wu</t>
-    </rPh>
-    <rPh sb="144" eb="145">
-      <t>zong'l</t>
-    </rPh>
-    <rPh sb="146" eb="147">
-      <t>shang'xian</t>
-    </rPh>
-    <rPh sb="149" eb="150">
-      <t>mei'ge</t>
-    </rPh>
-    <rPh sb="151" eb="152">
-      <t>dui'wu</t>
-    </rPh>
-    <rPh sb="153" eb="154">
-      <t>tong'shi</t>
-    </rPh>
-    <rPh sb="155" eb="156">
-      <t>rong'n</t>
-    </rPh>
-    <rPh sb="157" eb="158">
-      <t>de</t>
-    </rPh>
-    <rPh sb="158" eb="159">
-      <t>dan'wei</t>
-    </rPh>
-    <rPh sb="160" eb="161">
-      <t>shang'xian</t>
-    </rPh>
-    <rPh sb="162" eb="163">
-      <t>deng</t>
-    </rPh>
-    <rPh sb="163" eb="164">
-      <t>xiang'g</t>
-    </rPh>
-    <rPh sb="165" eb="166">
-      <t>luo'ji</t>
-    </rPh>
-    <rPh sb="167" eb="168">
-      <t>can'shu</t>
-    </rPh>
-    <rPh sb="170" eb="171">
-      <t>ying'g</t>
-    </rPh>
-    <rPh sb="172" eb="173">
-      <t>bao'zheng</t>
-    </rPh>
-    <rPh sb="174" eb="175">
-      <t>yi'dign</t>
-    </rPh>
-    <rPh sb="176" eb="177">
-      <t>de</t>
-    </rPh>
-    <rPh sb="177" eb="178">
-      <t>ling'huo'x</t>
-    </rPh>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>群体寻路/Multiple Units path finding</t>
     <rPh sb="0" eb="1">
       <t>qun'ti</t>
@@ -2282,6 +1824,616 @@
     <t>中</t>
     <rPh sb="0" eb="1">
       <t>zhong</t>
+    </rPh>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.框选之后按特定的组合键，能够进行编队，比如框选之后按ctrl+1，那么这次框选的游戏单位，将会被记录为1队，那么不管框选结束还是重新框选，当玩家再次按下1键时，会自动为玩家选择编队1的现存单位，并自动让这些单位变为已选状态;
+2.尽量保证功能的拓展性，比如组合键的可配置性，编队的队伍总量上限，每个队伍同时容纳的单位上限等相关逻辑参数，应该保证一定的灵活性。
+1.After finish selection and enter the specific key combination, game units can be teaming. Such press CTRL + 1, the game units that are selected, will be mark down as team1. Nomater ending selection or reselection, player can always call team 1 by press the key 1 key, automatically select the team1 for player.
+2.Ensure the function expansion flexibility, such as key combination of configurability, the maximum total team formation, each team cap logic parameters related to accommodate the unit.</t>
+    <rPh sb="2" eb="3">
+      <t>kuang'xuan</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>zhi'h</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>an</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>te'ding</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>de</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>zu'he'jian</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>neng</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>gou</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>jin'xing</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>bian'dui</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>bi'ru</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>kuang'xuan</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>zhi'h</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>an</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>na'm</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>zhe'ci</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>kuang'xuan</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>de</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>you'xi</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>dan'wei</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>jiang</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>hui</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>bei</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>ji'lu</t>
+    </rPh>
+    <rPh sb="52" eb="53">
+      <t>wei</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>dui</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>na'm</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>bu'guan</t>
+    </rPh>
+    <rPh sb="60" eb="61">
+      <t>kuang'x</t>
+    </rPh>
+    <rPh sb="62" eb="63">
+      <t>jie'shu</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>hai's</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>chogn'xin</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>kuang'x</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>dang</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t>wan'jia</t>
+    </rPh>
+    <rPh sb="74" eb="75">
+      <t>zai'ci</t>
+    </rPh>
+    <rPh sb="76" eb="77">
+      <t>an'xia</t>
+    </rPh>
+    <rPh sb="79" eb="80">
+      <t>jian</t>
+    </rPh>
+    <rPh sb="80" eb="81">
+      <t>shi</t>
+    </rPh>
+    <rPh sb="82" eb="83">
+      <t>hui</t>
+    </rPh>
+    <rPh sb="83" eb="84">
+      <t>zi'dong</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>wei</t>
+    </rPh>
+    <rPh sb="86" eb="87">
+      <t>wan'jia</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>xuan'z</t>
+    </rPh>
+    <rPh sb="90" eb="91">
+      <t>bian'dui</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>de</t>
+    </rPh>
+    <rPh sb="94" eb="95">
+      <t>xian'cun</t>
+    </rPh>
+    <rPh sb="96" eb="97">
+      <t>dan'wei</t>
+    </rPh>
+    <rPh sb="99" eb="100">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="100" eb="101">
+      <t>zi'dong</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>rtang</t>
+    </rPh>
+    <rPh sb="103" eb="104">
+      <t>zhe'x</t>
+    </rPh>
+    <rPh sb="105" eb="106">
+      <t>dan'wei</t>
+    </rPh>
+    <rPh sb="107" eb="108">
+      <t>bian'wei</t>
+    </rPh>
+    <rPh sb="109" eb="110">
+      <t>yi</t>
+    </rPh>
+    <rPh sb="110" eb="111">
+      <t>xuan</t>
+    </rPh>
+    <rPh sb="111" eb="112">
+      <t>zhuang'tai</t>
+    </rPh>
+    <rPh sb="117" eb="118">
+      <t>jin'l</t>
+    </rPh>
+    <rPh sb="119" eb="120">
+      <t>bao'zheng</t>
+    </rPh>
+    <rPh sb="121" eb="122">
+      <t>gogn'n</t>
+    </rPh>
+    <rPh sb="123" eb="124">
+      <t>de</t>
+    </rPh>
+    <rPh sb="124" eb="125">
+      <t>tuo'zhan</t>
+    </rPh>
+    <rPh sb="126" eb="127">
+      <t>xing</t>
+    </rPh>
+    <rPh sb="128" eb="129">
+      <t>bi'ru</t>
+    </rPh>
+    <rPh sb="130" eb="131">
+      <t>zu'he'j</t>
+    </rPh>
+    <rPh sb="133" eb="134">
+      <t>de</t>
+    </rPh>
+    <rPh sb="134" eb="135">
+      <t>ke'pei'zhi'xing</t>
+    </rPh>
+    <rPh sb="139" eb="140">
+      <t>bian'dui</t>
+    </rPh>
+    <rPh sb="141" eb="142">
+      <t>de</t>
+    </rPh>
+    <rPh sb="142" eb="143">
+      <t>dui'wu</t>
+    </rPh>
+    <rPh sb="144" eb="145">
+      <t>zong'l</t>
+    </rPh>
+    <rPh sb="146" eb="147">
+      <t>shang'xian</t>
+    </rPh>
+    <rPh sb="149" eb="150">
+      <t>mei'ge</t>
+    </rPh>
+    <rPh sb="151" eb="152">
+      <t>dui'wu</t>
+    </rPh>
+    <rPh sb="153" eb="154">
+      <t>tong'shi</t>
+    </rPh>
+    <rPh sb="155" eb="156">
+      <t>rong'n</t>
+    </rPh>
+    <rPh sb="157" eb="158">
+      <t>de</t>
+    </rPh>
+    <rPh sb="158" eb="159">
+      <t>dan'wei</t>
+    </rPh>
+    <rPh sb="160" eb="161">
+      <t>shang'xian</t>
+    </rPh>
+    <rPh sb="162" eb="163">
+      <t>deng</t>
+    </rPh>
+    <rPh sb="163" eb="164">
+      <t>xiang'g</t>
+    </rPh>
+    <rPh sb="165" eb="166">
+      <t>luo'ji</t>
+    </rPh>
+    <rPh sb="167" eb="168">
+      <t>can'shu</t>
+    </rPh>
+    <rPh sb="170" eb="171">
+      <t>ying'g</t>
+    </rPh>
+    <rPh sb="172" eb="173">
+      <t>bao'zheng</t>
+    </rPh>
+    <rPh sb="174" eb="175">
+      <t>yi'dign</t>
+    </rPh>
+    <rPh sb="176" eb="177">
+      <t>de</t>
+    </rPh>
+    <rPh sb="177" eb="178">
+      <t>ling'huo'x</t>
+    </rPh>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>战争迷雾/War Dense Fog</t>
+    <rPh sb="0" eb="1">
+      <t>zhan'zheng'mi'wu</t>
+    </rPh>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.框架应将项目基本Gameplay所需的基类、接口、委托等进行初步的代码实现；
+2.框架应具备适当的易用性，即框架的学习使用成本，不应占用过多的项目开发时间；
+3.在保证前2点的前提下，尽可能地减少框架本身的BUG，尽可能将框架设计的更加优雅，可拓展性、可维护性更高。
+1.The framework should carry out preliminary code implementation of the basic classes, interfaces, and delegates required for the basic Gameplay of the project;
+2.The framework should be easy to use, the cost of  framework learning should not take up too much project development time;
+3.In the premise of ensuring the first 2 points, you can reduce the BUG of the frame as much as possible, and make the frame more elegant, extensibility and maintainability as far as possible。
+</t>
+    <rPh sb="2" eb="3">
+      <t>kuang'j</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ying</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>jiang</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>xiang'mu</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ji'ben</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>suo'xu</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>de</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ji'lei</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>jie'kou</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>wei'tuo</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>deng</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>jin'xing</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>chu'bu</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>de</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>dai'm</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>shi'xian</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>kuang'j</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ying'ju'bei</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>shi'dang</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>de</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>yi'yong'xing</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>ji</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>kuang'j</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>de</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>xue'xi</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>shi'yong</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>cheng'b</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>bu'ying</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>zhan'yong</t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t>guo'gao</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>duo</t>
+    </rPh>
+    <rPh sb="72" eb="73">
+      <t>de</t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t>xiang'mu</t>
+    </rPh>
+    <rPh sb="75" eb="76">
+      <t>kai'fa</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>shi'jian</t>
+    </rPh>
+    <rPh sb="83" eb="84">
+      <t>zai</t>
+    </rPh>
+    <rPh sb="84" eb="85">
+      <t>bao'zheng</t>
+    </rPh>
+    <rPh sb="86" eb="87">
+      <t>qian</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>dian</t>
+    </rPh>
+    <rPh sb="89" eb="90">
+      <t>de</t>
+    </rPh>
+    <rPh sb="90" eb="91">
+      <t>qian'ti</t>
+    </rPh>
+    <rPh sb="92" eb="93">
+      <t>xia</t>
+    </rPh>
+    <rPh sb="94" eb="95">
+      <t>jin'ke'negn</t>
+    </rPh>
+    <rPh sb="97" eb="98">
+      <t>di</t>
+    </rPh>
+    <rPh sb="98" eb="99">
+      <t>jian'shao</t>
+    </rPh>
+    <rPh sb="100" eb="101">
+      <t>kuang'j</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>ben's</t>
+    </rPh>
+    <rPh sb="104" eb="105">
+      <t>de</t>
+    </rPh>
+    <rPh sb="109" eb="110">
+      <t>jin'ke'neng</t>
+    </rPh>
+    <rPh sb="112" eb="113">
+      <t>jiang</t>
+    </rPh>
+    <rPh sb="113" eb="114">
+      <t>kuang'j</t>
+    </rPh>
+    <rPh sb="115" eb="116">
+      <t>she'ji</t>
+    </rPh>
+    <rPh sb="117" eb="118">
+      <t>de</t>
+    </rPh>
+    <rPh sb="118" eb="119">
+      <t>geng'jia</t>
+    </rPh>
+    <rPh sb="120" eb="121">
+      <t>you'ya</t>
+    </rPh>
+    <rPh sb="123" eb="124">
+      <t>ke'tuo'zhan'x</t>
+    </rPh>
+    <rPh sb="128" eb="129">
+      <t>ke'wei'hu'x</t>
+    </rPh>
+    <rPh sb="132" eb="133">
+      <t>geng</t>
+    </rPh>
+    <rPh sb="133" eb="134">
+      <t>gao</t>
+    </rPh>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.每个己方以及友方单位，提供视野，建筑物、战斗兵种、生成单位提供的视野应该有所区别；
+2.综合计算总可见区域，并刷新小地图、主RTS摄像机显示；
+3.不在可见域内的游戏单位，应结合游戏设计逻辑进行相应的操作甄别筛选。
+1.Each party and friendly unit provides a vision of the view that the buildings, combat units, and generating units should provide;
+2.Each party and friendly unit provides a visual field of vision, which should be different from the view provided by the unit;
+3.The game units that are not in the visible should be support specific action with the game design logic.
+</t>
+    <rPh sb="2" eb="3">
+      <t>mei'ge</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ji'fang</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>yi'ji</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>you'fang</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>dan'wei</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ti'gong</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>shi'ye</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>jian'zhu'wu</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>zhan'dou</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>bing'zhogn</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>sheng'c</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>dan'wei</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ti'gong</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>de</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>shi'ye</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ying'g</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>you'suo'qu'b</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>zong'he</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>ji'suan</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>zong</t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t>ke'jian</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>qu'yu</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>bing</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>shua'xin</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>xiao'di'tu</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>zhu</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>she'xiang'ji</t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t>xian'shi</t>
+    </rPh>
+    <rPh sb="76" eb="77">
+      <t>bu'zai'ke'jian'yu</t>
+    </rPh>
+    <rPh sb="80" eb="81">
+      <t>yu</t>
+    </rPh>
+    <rPh sb="81" eb="82">
+      <t>nei</t>
+    </rPh>
+    <rPh sb="82" eb="83">
+      <t>de</t>
+    </rPh>
+    <rPh sb="83" eb="84">
+      <t>you'xi</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>dan'we</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>ying</t>
+    </rPh>
+    <rPh sb="89" eb="90">
+      <t>jie'he</t>
+    </rPh>
+    <rPh sb="91" eb="92">
+      <t>you'xi</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>she'ji</t>
+    </rPh>
+    <rPh sb="95" eb="96">
+      <t>luo'ji</t>
+    </rPh>
+    <rPh sb="97" eb="98">
+      <t>jin'xing</t>
+    </rPh>
+    <rPh sb="99" eb="100">
+      <t>xiang'ying</t>
+    </rPh>
+    <rPh sb="101" eb="102">
+      <t>de</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>cao'zuo</t>
+    </rPh>
+    <rPh sb="104" eb="105">
+      <t>zhen'bie</t>
+    </rPh>
+    <rPh sb="106" eb="107">
+      <t>shai'xuan</t>
     </rPh>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -2556,6 +2708,9 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <strike val="0"/>
@@ -2567,9 +2722,6 @@
         <color rgb="FFFF0000"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2727,8 +2879,8 @@
     <tableColumn id="10" name="任务权重/Task Priority" dataDxfId="2"/>
     <tableColumn id="4" name="开始日期/Start Date"/>
     <tableColumn id="5" name="到期日/End Date"/>
-    <tableColumn id="6" name="完成百分比" dataDxfId="0"/>
-    <tableColumn id="8" name="备注/Remarks" dataDxfId="1"/>
+    <tableColumn id="6" name="完成百分比" dataDxfId="1"/>
+    <tableColumn id="8" name="备注/Remarks" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Task List" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2948,8 +3100,8 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2992,7 +3144,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>5</v>
@@ -3012,14 +3164,14 @@
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="6">
         <v>43008</v>
@@ -3037,14 +3189,14 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="6">
         <v>43008</v>
@@ -3062,14 +3214,14 @@
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="6">
         <v>43008</v>
@@ -3087,13 +3239,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="6">
         <v>43008</v>
@@ -3111,13 +3263,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>18</v>
-      </c>
       <c r="E7" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="6">
         <v>43008</v>
@@ -3135,13 +3287,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>20</v>
-      </c>
       <c r="E8" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="6">
         <v>43008</v>
@@ -3159,13 +3311,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>23</v>
-      </c>
       <c r="E9" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="6">
         <v>43008</v>
@@ -3183,13 +3335,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="6">
         <v>43008</v>
@@ -3207,13 +3359,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>26</v>
-      </c>
       <c r="E11" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="6">
         <v>43008</v>
@@ -3231,13 +3383,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="6">
         <v>43008</v>
@@ -3255,13 +3407,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>32</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>34</v>
       </c>
       <c r="F13" s="6">
         <v>43008</v>
@@ -3274,8 +3426,16 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+    <row r="14" spans="1:9" ht="308" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="E14" s="26"/>
       <c r="H14" s="21"/>
       <c r="I14" s="2"/>

</xml_diff>